<commit_message>
update version to v0.4 structure: target=common options, value=options by case
</commit_message>
<xml_diff>
--- a/src/test/resources/addSelection/addSelection.xlsx
+++ b/src/test/resources/addSelection/addSelection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\addselection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\addSelection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE80B1A-0BFA-4E39-8860-15A4A556EE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B59529-54FB-403D-BEAC-0A39080490E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,7 +470,7 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>option</t>
+      <t>target</t>
     </r>
     <r>
       <rPr>
@@ -500,6 +500,92 @@
         <family val="3"/>
         <charset val="136"/>
       </rPr>
+      <t>"xpath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF067D17"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>//*[@id='issue_custom_field_values_31']"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF080808"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF871094"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF871094"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF871094"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF080808"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF067D17"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
       <t>"${company</t>
     </r>
     <r>
@@ -546,7 +632,27 @@
         <family val="3"/>
         <charset val="136"/>
       </rPr>
-      <t>"option"</t>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF871094"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF871094"/>
+        <rFont val="Sarasa Mono CL"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>"</t>
     </r>
     <r>
       <rPr>
@@ -587,92 +693,6 @@
         <charset val="136"/>
       </rPr>
       <t>}"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF080808"/>
-        <rFont val="Sarasa Mono CL"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF871094"/>
-        <rFont val="Sarasa Mono CL"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF871094"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>target</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF871094"/>
-        <rFont val="Sarasa Mono CL"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF080808"/>
-        <rFont val="Sarasa Mono CL"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Sarasa Mono CL"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>"xpath</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF067D17"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF067D17"/>
-        <rFont val="Sarasa Mono CL"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>//*[@id='issue_custom_field_values_31']"</t>
     </r>
     <r>
       <rPr>
@@ -1141,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1230,10 +1250,10 @@
         <v>17</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>13</v>
@@ -1263,10 +1283,10 @@
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>14</v>

</xml_diff>